<commit_message>
ml rfc file cleaned
</commit_message>
<xml_diff>
--- a/static/data/ml_score_card.xlsx
+++ b/static/data/ml_score_card.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meena\Dropbox\My PC (DESKTOP-UBVQVOT)\Desktop\MR_Food Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B5534D2-D9CC-4A0E-8BF6-74136A8FF8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E285174D-397D-48F8-BE21-97D07DC4B04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{CB7F3F66-6439-4580-A698-88CB5AA4E066}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CB7F3F66-6439-4580-A698-88CB5AA4E066}"/>
   </bookViews>
   <sheets>
     <sheet name="models_score" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Ada Boost Classifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Random Forest Classifier </t>
-  </si>
-  <si>
     <t>Testing Score</t>
   </si>
   <si>
@@ -130,6 +127,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Model</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Neural Network Optimized</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier  Optimized</t>
   </si>
 </sst>
 </file>
@@ -210,7 +219,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +247,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,19 +296,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -338,6 +362,28 @@
     <xf numFmtId="2" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,176 +705,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46638383-153A-4512-AE95-DB3F8EBC7BC9}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="37" customWidth="1"/>
+    <col min="4" max="5" width="12" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="38"/>
+    <col min="8" max="9" width="11.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:11" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="1:11" s="14" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="13"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+    </row>
+    <row r="3" spans="1:11" s="25" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-3.8758508688729801E-5</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>6.6971011510807296E-2</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>-3.8758508688729801E-5</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+    </row>
+    <row r="7" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.70645269140755595</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+    </row>
+    <row r="8" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.73604145770645202</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+    </row>
+    <row r="9" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.64799955421820998</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.76161818789702396</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.68722835172183205</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.74852334782124097</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0.77671904602696895</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="27">
+        <v>0.81934371656164495</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-3.8758508688729801E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6.2360117996025102E-2</v>
-      </c>
-      <c r="C5" s="6">
-        <v>6.6971011510807296E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>-3.8758508688729801E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.70486291700720705</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.70645269140755595</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.81296901701463697</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.73604145770645202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0.64651905787948505</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0.64799955421820998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.76523144364365803</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.76161818789702396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.68722835172183205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.74782673304108704</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.74852334782124097</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.99996285013745401</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0.77671904602696895</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="B15" s="29">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
@@ -843,211 +1000,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEEDE29-D111-4072-A019-6CF9765A43D2}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" style="17" customWidth="1"/>
-    <col min="3" max="5" width="12.6328125" style="16" customWidth="1"/>
-    <col min="6" max="11" width="12.6328125" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="17"/>
+    <col min="1" max="1" width="27.6328125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" style="14" customWidth="1"/>
+    <col min="3" max="5" width="12.6328125" style="13" customWidth="1"/>
+    <col min="6" max="11" width="12.6328125" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="A1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="31" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="11" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="7">
+        <v>0.99996285013745401</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.77671904602696895</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.71</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.91</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10">
-        <v>0.99996285013745401</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.77671904602696895</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.78</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0.71</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0.91</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.59</v>
-      </c>
-      <c r="K4" s="10">
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.84407323742717799</v>
+      </c>
+      <c r="E5" s="7">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="11" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="F5" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.84407323742717799</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.85</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.76</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="C6" s="7">
+        <v>0.99998018389346799</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.84169539888241496</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="G6" s="8">
         <v>0.87</v>
       </c>
-      <c r="H5" s="10">
-        <v>0.65</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="H6" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="I6" s="10">
         <v>0.92</v>
       </c>
-      <c r="J5" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="11" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="J6" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="10">
-        <v>0.99998018389346799</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.84169539888241496</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0.87</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0.63</v>
-      </c>
-      <c r="I6" s="13">
-        <v>0.92</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0.68</v>
-      </c>
-      <c r="K6" s="11">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>0.83172162333544697</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>0.81934371656164495</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>0.82</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>0.77</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>0.83</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <v>0.49</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="10">
         <v>0.94</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>0.6</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="8">
         <v>0.88</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>